<commit_message>
some dec 2017 changes
</commit_message>
<xml_diff>
--- a/lifehist/2017_12_08 GLMM tables.xlsx
+++ b/lifehist/2017_12_08 GLMM tables.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="161">
   <si>
     <t>Estimate</t>
   </si>
@@ -450,6 +450,66 @@
   </si>
   <si>
     <t>Lat_group * Temp_let + (1 | State) + (1 | Family)</t>
+  </si>
+  <si>
+    <t>coxph(formula = Surv(time, Death_stat) ~ Biome + Temp_num, data = lifehistshort)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  n= 3430, number of events= 2653 </t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>Signif. codes:  0 ‘***’ 0.001 ‘**’ 0.01 ‘*’ 0.05 ‘.’ 0.1 ‘ ’ 1</t>
+  </si>
+  <si>
+    <t>Concordance= 0.769  (se = 0.007 )</t>
+  </si>
+  <si>
+    <t>Rsquare= 0.358   (max possible= 1 )</t>
+  </si>
+  <si>
+    <t>Likelihood ratio test= 1518  on 3 df,   p=0</t>
+  </si>
+  <si>
+    <t>Wald test            = 1431  on 3 df,   p=0</t>
+  </si>
+  <si>
+    <t>Score (logrank) test = 1516  on 3 df,   p=0</t>
+  </si>
+  <si>
+    <t>&lt;2e-16</t>
+  </si>
+  <si>
+    <t>Temp_num</t>
+  </si>
+  <si>
+    <t>exp(-coef)</t>
+  </si>
+  <si>
+    <t>lower .95</t>
+  </si>
+  <si>
+    <t>upper .95</t>
+  </si>
+  <si>
+    <t>Predictor</t>
+  </si>
+  <si>
+    <t>Exp(coef)</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Standard error</t>
+  </si>
+  <si>
+    <t>Coef</t>
   </si>
 </sst>
 </file>
@@ -489,11 +549,13 @@
       <sz val="15"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="15"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -686,23 +748,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -724,15 +774,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -749,9 +790,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2202,24 +2269,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="7:30" x14ac:dyDescent="0.4">
-      <c r="R3" s="5" t="s">
+      <c r="R3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="7"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="22"/>
     </row>
     <row r="4" spans="7:30" x14ac:dyDescent="0.4">
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2" t="s">
         <v>0</v>
@@ -2234,14 +2301,14 @@
         <v>3</v>
       </c>
       <c r="W4" s="2"/>
-      <c r="Y4" s="4" t="s">
+      <c r="Y4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="19"/>
     </row>
     <row r="5" spans="7:30" x14ac:dyDescent="0.4">
       <c r="J5" s="2"/>
@@ -2784,14 +2851,14 @@
       <c r="AD14" s="2"/>
     </row>
     <row r="15" spans="7:30" x14ac:dyDescent="0.4">
-      <c r="J15" s="4" t="s">
+      <c r="J15" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
       <c r="R15" s="2" t="s">
         <v>16</v>
       </c>
@@ -2810,14 +2877,14 @@
       <c r="W15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Y15" s="4" t="s">
+      <c r="Y15" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
-      <c r="AB15" s="4"/>
-      <c r="AC15" s="4"/>
-      <c r="AD15" s="4"/>
+      <c r="Z15" s="19"/>
+      <c r="AA15" s="19"/>
+      <c r="AB15" s="19"/>
+      <c r="AC15" s="19"/>
+      <c r="AD15" s="19"/>
     </row>
     <row r="16" spans="7:30" x14ac:dyDescent="0.4">
       <c r="G16" s="1" t="s">
@@ -2856,7 +2923,7 @@
         <v>16.840599999999998</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" ref="H17:I32" si="0">1/H17</f>
+        <f t="shared" ref="I17:I24" si="0">1/H17</f>
         <v>5.9380307114948405E-2</v>
       </c>
       <c r="R17" s="2" t="s">
@@ -3064,14 +3131,14 @@
         <f t="shared" si="0"/>
         <v>5.8647242699884472E-2</v>
       </c>
-      <c r="R24" s="4" t="s">
+      <c r="R24" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="19"/>
+      <c r="V24" s="19"/>
+      <c r="W24" s="19"/>
     </row>
     <row r="25" spans="6:23" x14ac:dyDescent="0.4">
       <c r="F25" s="1" t="s">
@@ -3203,106 +3270,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.6">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="19.5" x14ac:dyDescent="0.6">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="8">
         <v>-2.8639999999999999</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="8">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="19.5" x14ac:dyDescent="0.6">
-      <c r="A3" s="16"/>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="8">
         <v>-3.028</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="8">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="19.5" x14ac:dyDescent="0.6">
-      <c r="A4" s="16"/>
-      <c r="B4" s="11" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="8">
         <v>-8.7420000000000009</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="8">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="19.5" x14ac:dyDescent="0.6">
-      <c r="A5" s="17"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="8">
         <v>-9.2230000000000008</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="8">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="19.5" x14ac:dyDescent="0.6">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="8">
         <v>-10.7</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="8">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.6">
-      <c r="A7" s="17"/>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="25"/>
+      <c r="B7" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="8">
         <v>-10.795999999999999</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="8">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="10">
         <v>-22.611000000000001</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="10">
         <v>11</v>
       </c>
     </row>
@@ -3317,21 +3384,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B38D0DA5-94E5-4B4C-8F1E-8A5A51406A71}">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:G29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39:J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="38.73046875" customWidth="1"/>
     <col min="6" max="6" width="7.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.1328125" customWidth="1"/>
+    <col min="10" max="10" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="5" t="s">
         <v>90</v>
       </c>
       <c r="B1" t="s">
@@ -3351,7 +3420,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B2" t="s">
@@ -3359,10 +3428,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="8"/>
+      <c r="A3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="9"/>
+      <c r="A4" s="5"/>
       <c r="B4" t="s">
         <v>98</v>
       </c>
@@ -3380,7 +3449,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B5">
@@ -3400,7 +3469,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B6">
@@ -3420,7 +3489,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B7">
@@ -3440,7 +3509,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B8">
@@ -3460,7 +3529,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B9" t="s">
@@ -3480,7 +3549,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="5" t="s">
         <v>105</v>
       </c>
       <c r="B10" t="s">
@@ -3500,7 +3569,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B11" t="s">
@@ -3515,12 +3584,12 @@
       <c r="E11">
         <v>-5.96</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="14">
         <v>2.5000000000000001E-9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="5" t="s">
         <v>105</v>
       </c>
       <c r="B12" t="s">
@@ -3540,10 +3609,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="8"/>
+      <c r="A13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="5" t="s">
         <v>109</v>
       </c>
       <c r="B14" t="s">
@@ -3554,7 +3623,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="5" t="s">
         <v>112</v>
       </c>
       <c r="B15" t="s">
@@ -3584,7 +3653,7 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="9"/>
+      <c r="H20" s="5"/>
       <c r="I20" t="s">
         <v>98</v>
       </c>
@@ -3602,23 +3671,23 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A21" s="22"/>
-      <c r="B21" s="23" t="s">
+      <c r="A21" s="15"/>
+      <c r="B21" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="E21" s="23" t="s">
+      <c r="E21" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="H21" s="5" t="s">
         <v>116</v>
       </c>
       <c r="I21">
@@ -3641,25 +3710,25 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="B22" s="23">
+      <c r="B22" s="16">
         <v>-0.377</v>
       </c>
-      <c r="C22" s="23">
+      <c r="C22" s="16">
         <v>0.68589999999999995</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="16">
         <v>9.7500000000000003E-2</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="16">
         <v>-3.87</v>
       </c>
-      <c r="F22" s="24">
+      <c r="F22" s="17">
         <v>1.1E-4</v>
       </c>
-      <c r="H22" s="9" t="s">
+      <c r="H22" s="5" t="s">
         <v>117</v>
       </c>
       <c r="I22">
@@ -3682,25 +3751,25 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B23" s="23">
+      <c r="B23" s="16">
         <v>-0.99360000000000004</v>
       </c>
-      <c r="C23" s="23">
+      <c r="C23" s="16">
         <v>0.37019999999999997</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="16">
         <v>9.8500000000000004E-2</v>
       </c>
-      <c r="E23" s="23">
+      <c r="E23" s="16">
         <v>-10.09</v>
       </c>
-      <c r="F23" s="24" t="s">
+      <c r="F23" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H23" s="9" t="s">
+      <c r="H23" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I23">
@@ -3723,25 +3792,25 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="16">
         <v>1.3096000000000001</v>
       </c>
-      <c r="C24" s="23">
+      <c r="C24" s="16">
         <v>3.7048000000000001</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="16">
         <v>5.6099999999999997E-2</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="16">
         <v>23.33</v>
       </c>
-      <c r="F24" s="24" t="s">
+      <c r="F24" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="H24" s="5" t="s">
         <v>8</v>
       </c>
       <c r="I24">
@@ -3764,25 +3833,25 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="23">
+      <c r="B25" s="16">
         <v>2.1396999999999999</v>
       </c>
-      <c r="C25" s="23">
+      <c r="C25" s="16">
         <v>8.4966000000000008</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="16">
         <v>6.3299999999999995E-2</v>
       </c>
-      <c r="E25" s="23">
+      <c r="E25" s="16">
         <v>33.79</v>
       </c>
-      <c r="F25" s="24" t="s">
+      <c r="F25" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="H25" s="5" t="s">
         <v>118</v>
       </c>
       <c r="I25">
@@ -3797,7 +3866,7 @@
       <c r="L25">
         <v>-4.3419999999999996</v>
       </c>
-      <c r="M25" s="21">
+      <c r="M25" s="14">
         <v>1.4100000000000001E-5</v>
       </c>
       <c r="N25" t="s">
@@ -3805,25 +3874,25 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="23">
+      <c r="B26" s="16">
         <v>-0.52610000000000001</v>
       </c>
-      <c r="C26" s="23">
+      <c r="C26" s="16">
         <v>0.59089999999999998</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="16">
         <v>0.13930000000000001</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="16">
         <v>-3.78</v>
       </c>
-      <c r="F26" s="24">
+      <c r="F26" s="17">
         <v>1.6000000000000001E-4</v>
       </c>
-      <c r="H26" s="9" t="s">
+      <c r="H26" s="5" t="s">
         <v>119</v>
       </c>
       <c r="I26">
@@ -3843,25 +3912,25 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="B27" s="23">
+      <c r="B27" s="16">
         <v>-1.4999999999999999E-2</v>
       </c>
-      <c r="C27" s="23">
+      <c r="C27" s="16">
         <v>0.98509999999999998</v>
       </c>
-      <c r="D27" s="23">
+      <c r="D27" s="16">
         <v>0.13900000000000001</v>
       </c>
-      <c r="E27" s="23">
+      <c r="E27" s="16">
         <v>-0.11</v>
       </c>
-      <c r="F27" s="23">
+      <c r="F27" s="16">
         <v>0.91413999999999995</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="H27" s="5" t="s">
         <v>120</v>
       </c>
       <c r="I27">
@@ -3876,7 +3945,7 @@
       <c r="L27">
         <v>-5.6509999999999998</v>
       </c>
-      <c r="M27" s="21">
+      <c r="M27" s="14">
         <v>1.6000000000000001E-8</v>
       </c>
       <c r="N27" t="s">
@@ -3884,25 +3953,25 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="B28" s="23">
+      <c r="B28" s="16">
         <v>-0.98499999999999999</v>
       </c>
-      <c r="C28" s="23">
+      <c r="C28" s="16">
         <v>0.37340000000000001</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="16">
         <v>0.14779999999999999</v>
       </c>
-      <c r="E28" s="23">
+      <c r="E28" s="16">
         <v>-6.67</v>
       </c>
-      <c r="F28" s="25">
+      <c r="F28" s="18">
         <v>2.6000000000000001E-11</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="H28" s="5" t="s">
         <v>121</v>
       </c>
       <c r="I28">
@@ -3922,30 +3991,30 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="B29" s="23">
+      <c r="B29" s="16">
         <v>-1.819</v>
       </c>
-      <c r="C29" s="23">
+      <c r="C29" s="16">
         <v>0.16220000000000001</v>
       </c>
-      <c r="D29" s="23">
+      <c r="D29" s="16">
         <v>0.20480000000000001</v>
       </c>
-      <c r="E29" s="23">
+      <c r="E29" s="16">
         <v>-8.8800000000000008</v>
       </c>
-      <c r="F29" s="24" t="s">
+      <c r="F29" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A30" s="8"/>
+      <c r="A30" s="4"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B31" t="s">
@@ -3956,11 +4025,293 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="5" t="s">
         <v>125</v>
       </c>
       <c r="B32">
         <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A35" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A36" s="4"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A37" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A38" s="4"/>
+      <c r="H38" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="I38" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="J38" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="K38" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="L38" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="M38" s="29" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A39" s="5"/>
+      <c r="B39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" t="s">
+        <v>101</v>
+      </c>
+      <c r="F39" t="s">
+        <v>3</v>
+      </c>
+      <c r="H39" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="I39" s="16">
+        <v>-0.86450499999999997</v>
+      </c>
+      <c r="J39" s="27">
+        <v>0.42130000000000001</v>
+      </c>
+      <c r="K39" s="27">
+        <v>5.9659999999999998E-2</v>
+      </c>
+      <c r="L39" s="27">
+        <v>-14.49</v>
+      </c>
+      <c r="M39" s="29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A40" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40">
+        <v>-0.86450499999999997</v>
+      </c>
+      <c r="C40">
+        <v>0.42126000000000002</v>
+      </c>
+      <c r="D40">
+        <v>5.9659999999999998E-2</v>
+      </c>
+      <c r="E40">
+        <v>-14.49</v>
+      </c>
+      <c r="F40" t="s">
+        <v>150</v>
+      </c>
+      <c r="G40" t="s">
+        <v>6</v>
+      </c>
+      <c r="H40" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="I40" s="16">
+        <v>-1.433676</v>
+      </c>
+      <c r="J40" s="27">
+        <v>0.2384</v>
+      </c>
+      <c r="K40" s="27">
+        <v>6.5254999999999994E-2</v>
+      </c>
+      <c r="L40" s="27">
+        <v>-21.97</v>
+      </c>
+      <c r="M40" s="29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A41" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41">
+        <v>-1.433676</v>
+      </c>
+      <c r="C41">
+        <v>0.238431</v>
+      </c>
+      <c r="D41">
+        <v>6.5254999999999994E-2</v>
+      </c>
+      <c r="E41">
+        <v>-21.97</v>
+      </c>
+      <c r="F41" t="s">
+        <v>150</v>
+      </c>
+      <c r="G41" t="s">
+        <v>6</v>
+      </c>
+      <c r="H41" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="I41" s="16">
+        <v>0.22845299999999999</v>
+      </c>
+      <c r="J41" s="27">
+        <v>1.2566999999999999</v>
+      </c>
+      <c r="K41" s="27">
+        <v>6.8490000000000001E-3</v>
+      </c>
+      <c r="L41" s="27">
+        <v>33.36</v>
+      </c>
+      <c r="M41" s="29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A42" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B42">
+        <v>0.22845299999999999</v>
+      </c>
+      <c r="C42">
+        <v>1.2566550000000001</v>
+      </c>
+      <c r="D42">
+        <v>6.8490000000000001E-3</v>
+      </c>
+      <c r="E42">
+        <v>33.36</v>
+      </c>
+      <c r="F42" t="s">
+        <v>150</v>
+      </c>
+      <c r="G42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A43" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A44" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A46" s="5"/>
+      <c r="B46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46" t="s">
+        <v>152</v>
+      </c>
+      <c r="D46" t="s">
+        <v>153</v>
+      </c>
+      <c r="E46" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A47" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B47">
+        <v>0.42130000000000001</v>
+      </c>
+      <c r="C47">
+        <v>2.3738000000000001</v>
+      </c>
+      <c r="D47">
+        <v>0.37480000000000002</v>
+      </c>
+      <c r="E47">
+        <v>0.47349999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A48" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B48">
+        <v>0.2384</v>
+      </c>
+      <c r="C48">
+        <v>4.1940999999999997</v>
+      </c>
+      <c r="D48">
+        <v>0.20979999999999999</v>
+      </c>
+      <c r="E48">
+        <v>0.27100000000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A49" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B49">
+        <v>1.2566999999999999</v>
+      </c>
+      <c r="C49">
+        <v>0.79579999999999995</v>
+      </c>
+      <c r="D49">
+        <v>1.2399</v>
+      </c>
+      <c r="E49">
+        <v>1.2736000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A50" s="4"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A51" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A52" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A53" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A54" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A55" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -3988,7 +4339,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="9"/>
+      <c r="A1" s="5"/>
       <c r="B1" t="s">
         <v>33</v>
       </c>
@@ -4000,7 +4351,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B2">
@@ -4009,12 +4360,12 @@
       <c r="C2">
         <v>-18656.830000000002</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B3">
@@ -4023,12 +4374,12 @@
       <c r="C3">
         <v>-18655.36</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B4">
@@ -4037,12 +4388,12 @@
       <c r="C4">
         <v>-18650.5</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B5">
@@ -4051,12 +4402,12 @@
       <c r="C5">
         <v>-18650.47</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B6">
@@ -4065,12 +4416,12 @@
       <c r="C6">
         <v>-18617.88</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B7">
@@ -4079,12 +4430,12 @@
       <c r="C7">
         <v>-18617.13</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B8">
@@ -4093,12 +4444,12 @@
       <c r="C8">
         <v>-16935.09</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B9">
@@ -4107,12 +4458,12 @@
       <c r="C9">
         <v>-16934.98</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" s="9"/>
+      <c r="A13" s="5"/>
       <c r="B13" t="s">
         <v>33</v>
       </c>
@@ -4121,7 +4472,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B14">
@@ -4130,12 +4481,12 @@
       <c r="C14">
         <v>-16929.91</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B15">
@@ -4144,12 +4495,12 @@
       <c r="C15">
         <v>-16930.09</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B16">
@@ -4158,12 +4509,12 @@
       <c r="C16">
         <v>-18643.55</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="5" t="s">
         <v>55</v>
       </c>
       <c r="B17">
@@ -4172,12 +4523,12 @@
       <c r="C17">
         <v>-18648.330000000002</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B18">
@@ -4186,12 +4537,12 @@
       <c r="C18">
         <v>-18610.14</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="5" t="s">
         <v>57</v>
       </c>
       <c r="B19">
@@ -4200,12 +4551,12 @@
       <c r="C19">
         <v>-18610.849999999999</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B20">
@@ -4214,12 +4565,12 @@
       <c r="C20">
         <v>-18643.54</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="5" t="s">
         <v>59</v>
       </c>
       <c r="B21">
@@ -4228,12 +4579,12 @@
       <c r="C21">
         <v>-18649.79</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="5" t="s">
         <v>60</v>
       </c>
       <c r="B22">
@@ -4247,7 +4598,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" s="9"/>
+      <c r="A27" s="5"/>
       <c r="B27" t="s">
         <v>33</v>
       </c>
@@ -4259,7 +4610,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="5" t="s">
         <v>134</v>
       </c>
       <c r="B28">
@@ -4273,7 +4624,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="5" t="s">
         <v>129</v>
       </c>
       <c r="B29">
@@ -4282,12 +4633,12 @@
       <c r="C29">
         <v>13256.69</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="5" t="s">
         <v>133</v>
       </c>
       <c r="B30">
@@ -4296,12 +4647,12 @@
       <c r="C30">
         <v>13256.89</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="5" t="s">
         <v>130</v>
       </c>
       <c r="B31">
@@ -4310,12 +4661,12 @@
       <c r="C31">
         <v>13259.97</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="5" t="s">
         <v>128</v>
       </c>
       <c r="B32">
@@ -4324,12 +4675,12 @@
       <c r="C32">
         <v>13262.2</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="5" t="s">
         <v>132</v>
       </c>
       <c r="B33">
@@ -4338,12 +4689,12 @@
       <c r="C33">
         <v>13262.28</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="5" t="s">
         <v>131</v>
       </c>
       <c r="B34">
@@ -4352,12 +4703,12 @@
       <c r="C34">
         <v>13262.32</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="5" t="s">
         <v>127</v>
       </c>
       <c r="B35">
@@ -4366,12 +4717,12 @@
       <c r="C35">
         <v>13873.11</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="5" t="s">
         <v>126</v>
       </c>
       <c r="B36">
@@ -4380,62 +4731,62 @@
       <c r="C36">
         <v>13875.69</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B40" s="24" t="s">
+      <c r="B40" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C40" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D40" s="24" t="s">
+      <c r="D40" s="17" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B41" s="23">
+      <c r="B41" s="16">
         <v>12</v>
       </c>
-      <c r="C41" s="23">
+      <c r="C41" s="16">
         <v>13256.69</v>
       </c>
-      <c r="D41" s="22" t="s">
+      <c r="D41" s="15" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B42" s="23">
+      <c r="B42" s="16">
         <v>11</v>
       </c>
-      <c r="C42" s="23">
+      <c r="C42" s="16">
         <v>13256.89</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="D42" s="15" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B43" s="23">
+      <c r="B43" s="16">
         <v>12</v>
       </c>
-      <c r="C43" s="23">
+      <c r="C43" s="16">
         <v>13262.2</v>
       </c>
-      <c r="D43" s="22" t="s">
+      <c r="D43" s="15" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B44" s="23">
+      <c r="B44" s="16">
         <v>11</v>
       </c>
-      <c r="C44" s="23">
+      <c r="C44" s="16">
         <v>13262.28</v>
       </c>
-      <c r="D44" s="22" t="s">
+      <c r="D44" s="15" t="s">
         <v>140</v>
       </c>
     </row>

</xml_diff>